<commit_message>
fix outfall bug, update documentation
</commit_message>
<xml_diff>
--- a/test_data/swmm_data/gisswmm_curves.xlsx
+++ b/test_data/swmm_data/gisswmm_curves.xlsx
@@ -4,17 +4,17 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pump2" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Rating" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Storage" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Weir" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Pump1" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Pump3" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Pump4" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Tidal" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Tidal" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Weir" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Pump1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Pump3" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Pump4" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="Control" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="Diversion" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="Shape" sheetId="11" state="visible" r:id="rId11"/>
@@ -63,18 +63,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -536,7 +536,7 @@
       <c r="D6" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -577,7 +577,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -618,7 +618,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -757,7 +757,7 @@
       <c r="D8" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1106,11 +1106,136 @@
       <c r="D23" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Hour_of_Day</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Stage</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>tdc_1</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>tdc_1</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>tdc_1</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="D4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>tdc_1</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>tdc_1</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>tdc_1</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1203,48 +1328,7 @@
       <c r="D5" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Volume</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Flow</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Notes</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1270,7 +1354,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Head</t>
+          <t>Volume</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -1285,7 +1369,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1311,7 +1395,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Depth</t>
+          <t>Head</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -1326,7 +1410,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1352,12 +1436,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Hour_of_Day</t>
+          <t>Depth</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Stage</t>
+          <t>Flow</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -1367,7 +1451,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1408,6 +1492,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>